<commit_message>
converted is hashed from numeric to logical
</commit_message>
<xml_diff>
--- a/results/tables/paper/scRNA-seq_qc_table_by_time_point.xlsx
+++ b/results/tables/paper/scRNA-seq_qc_table_by_time_point.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
   <si>
     <t xml:space="preserve">Case</t>
   </si>
@@ -65,6 +65,9 @@
     <t xml:space="preserve">Chromium v3</t>
   </si>
   <si>
+    <t xml:space="preserve">TRUE</t>
+  </si>
+  <si>
     <t xml:space="preserve">T2</t>
   </si>
   <si>
@@ -102,6 +105,9 @@
   </si>
   <si>
     <t xml:space="preserve">BCLLATLAS_29</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FALSE</t>
   </si>
   <si>
     <t xml:space="preserve">LN</t>
@@ -508,8 +514,8 @@
       <c r="F2" t="s">
         <v>16</v>
       </c>
-      <c r="G2" t="b">
-        <v>1</v>
+      <c r="G2" t="s">
+        <v>17</v>
       </c>
       <c r="H2" t="n">
         <v>245</v>
@@ -529,10 +535,10 @@
         <v>11</v>
       </c>
       <c r="B3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D3" t="s">
         <v>14</v>
@@ -543,8 +549,8 @@
       <c r="F3" t="s">
         <v>16</v>
       </c>
-      <c r="G3" t="b">
-        <v>1</v>
+      <c r="G3" t="s">
+        <v>17</v>
       </c>
       <c r="H3" t="n">
         <v>65</v>
@@ -564,10 +570,10 @@
         <v>11</v>
       </c>
       <c r="B4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D4" t="s">
         <v>14</v>
@@ -578,8 +584,8 @@
       <c r="F4" t="s">
         <v>16</v>
       </c>
-      <c r="G4" t="b">
-        <v>1</v>
+      <c r="G4" t="s">
+        <v>17</v>
       </c>
       <c r="H4" t="n">
         <v>1626</v>
@@ -599,10 +605,10 @@
         <v>11</v>
       </c>
       <c r="B5" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C5" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D5" t="s">
         <v>14</v>
@@ -613,8 +619,8 @@
       <c r="F5" t="s">
         <v>16</v>
       </c>
-      <c r="G5" t="b">
-        <v>1</v>
+      <c r="G5" t="s">
+        <v>17</v>
       </c>
       <c r="H5" t="n">
         <v>2529</v>
@@ -634,10 +640,10 @@
         <v>11</v>
       </c>
       <c r="B6" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C6" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D6" t="s">
         <v>14</v>
@@ -648,8 +654,8 @@
       <c r="F6" t="s">
         <v>16</v>
       </c>
-      <c r="G6" t="b">
-        <v>1</v>
+      <c r="G6" t="s">
+        <v>17</v>
       </c>
       <c r="H6" t="n">
         <v>1320</v>
@@ -666,7 +672,7 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B7" t="s">
         <v>12</v>
@@ -683,8 +689,8 @@
       <c r="F7" t="s">
         <v>16</v>
       </c>
-      <c r="G7" t="b">
-        <v>1</v>
+      <c r="G7" t="s">
+        <v>17</v>
       </c>
       <c r="H7" t="n">
         <v>330</v>
@@ -701,13 +707,13 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B8" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C8" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D8" t="s">
         <v>14</v>
@@ -718,8 +724,8 @@
       <c r="F8" t="s">
         <v>16</v>
       </c>
-      <c r="G8" t="b">
-        <v>1</v>
+      <c r="G8" t="s">
+        <v>17</v>
       </c>
       <c r="H8" t="n">
         <v>2800</v>
@@ -736,13 +742,13 @@
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B9" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C9" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D9" t="s">
         <v>14</v>
@@ -753,8 +759,8 @@
       <c r="F9" t="s">
         <v>16</v>
       </c>
-      <c r="G9" t="b">
-        <v>1</v>
+      <c r="G9" t="s">
+        <v>17</v>
       </c>
       <c r="H9" t="n">
         <v>1368</v>
@@ -771,13 +777,13 @@
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B10" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C10" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D10" t="s">
         <v>14</v>
@@ -788,8 +794,8 @@
       <c r="F10" t="s">
         <v>16</v>
       </c>
-      <c r="G10" t="b">
-        <v>1</v>
+      <c r="G10" t="s">
+        <v>17</v>
       </c>
       <c r="H10" t="n">
         <v>955</v>
@@ -806,14 +812,14 @@
     </row>
     <row r="11">
       <c r="A11" t="s">
+        <v>26</v>
+      </c>
+      <c r="B11" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11" t="s">
         <v>25</v>
       </c>
-      <c r="B11" t="s">
-        <v>23</v>
-      </c>
-      <c r="C11" t="s">
-        <v>24</v>
-      </c>
       <c r="D11" t="s">
         <v>14</v>
       </c>
@@ -823,8 +829,8 @@
       <c r="F11" t="s">
         <v>16</v>
       </c>
-      <c r="G11" t="b">
-        <v>1</v>
+      <c r="G11" t="s">
+        <v>17</v>
       </c>
       <c r="H11" t="n">
         <v>1831</v>
@@ -841,16 +847,16 @@
     </row>
     <row r="12">
       <c r="A12" t="s">
+        <v>29</v>
+      </c>
+      <c r="B12" t="s">
+        <v>18</v>
+      </c>
+      <c r="C12" t="s">
         <v>28</v>
       </c>
-      <c r="B12" t="s">
-        <v>17</v>
-      </c>
-      <c r="C12" t="s">
-        <v>27</v>
-      </c>
       <c r="D12" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E12" t="s">
         <v>15</v>
@@ -858,8 +864,8 @@
       <c r="F12" t="s">
         <v>16</v>
       </c>
-      <c r="G12" t="b">
-        <v>0</v>
+      <c r="G12" t="s">
+        <v>31</v>
       </c>
       <c r="H12" t="n">
         <v>4119</v>
@@ -876,25 +882,25 @@
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B13" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C13" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D13" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E13" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="F13" t="s">
         <v>16</v>
       </c>
-      <c r="G13" t="b">
-        <v>0</v>
+      <c r="G13" t="s">
+        <v>31</v>
       </c>
       <c r="H13" t="n">
         <v>566</v>
@@ -911,25 +917,25 @@
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B14" t="s">
         <v>12</v>
       </c>
       <c r="C14" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D14" t="s">
         <v>14</v>
       </c>
       <c r="E14" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="F14" t="s">
         <v>16</v>
       </c>
-      <c r="G14" t="b">
-        <v>1</v>
+      <c r="G14" t="s">
+        <v>17</v>
       </c>
       <c r="H14" t="n">
         <v>4246</v>
@@ -946,25 +952,25 @@
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B15" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C15" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D15" t="s">
         <v>14</v>
       </c>
       <c r="E15" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="F15" t="s">
         <v>16</v>
       </c>
-      <c r="G15" t="b">
-        <v>1</v>
+      <c r="G15" t="s">
+        <v>17</v>
       </c>
       <c r="H15" t="n">
         <v>1176</v>
@@ -981,25 +987,25 @@
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B16" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C16" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D16" t="s">
         <v>14</v>
       </c>
       <c r="E16" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="F16" t="s">
         <v>16</v>
       </c>
-      <c r="G16" t="b">
-        <v>1</v>
+      <c r="G16" t="s">
+        <v>17</v>
       </c>
       <c r="H16" t="n">
         <v>641</v>
@@ -1016,7 +1022,7 @@
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B17" t="s">
         <v>12</v>
@@ -1025,16 +1031,16 @@
         <v>13</v>
       </c>
       <c r="D17" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="E17" t="s">
         <v>15</v>
       </c>
       <c r="F17" t="s">
-        <v>35</v>
-      </c>
-      <c r="G17" t="b">
-        <v>0</v>
+        <v>37</v>
+      </c>
+      <c r="G17" t="s">
+        <v>31</v>
       </c>
       <c r="H17" t="n">
         <v>250</v>
@@ -1051,25 +1057,25 @@
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B18" t="s">
         <v>12</v>
       </c>
       <c r="C18" t="s">
+        <v>38</v>
+      </c>
+      <c r="D18" t="s">
         <v>36</v>
       </c>
-      <c r="D18" t="s">
-        <v>34</v>
-      </c>
       <c r="E18" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="F18" t="s">
-        <v>35</v>
-      </c>
-      <c r="G18" t="b">
-        <v>0</v>
+        <v>37</v>
+      </c>
+      <c r="G18" t="s">
+        <v>31</v>
       </c>
       <c r="H18" t="n">
         <v>268</v>
@@ -1086,25 +1092,25 @@
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B19" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C19" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D19" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="E19" t="s">
         <v>15</v>
       </c>
       <c r="F19" t="s">
-        <v>35</v>
-      </c>
-      <c r="G19" t="b">
-        <v>0</v>
+        <v>37</v>
+      </c>
+      <c r="G19" t="s">
+        <v>31</v>
       </c>
       <c r="H19" t="n">
         <v>253</v>
@@ -1121,25 +1127,25 @@
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B20" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C20" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D20" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="E20" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="F20" t="s">
-        <v>35</v>
-      </c>
-      <c r="G20" t="b">
-        <v>0</v>
+        <v>37</v>
+      </c>
+      <c r="G20" t="s">
+        <v>31</v>
       </c>
       <c r="H20" t="n">
         <v>212</v>

</xml_diff>